<commit_message>
edit date di wbs header dan order ascending
</commit_message>
<xml_diff>
--- a/jembatan Beton Coba 1.xlsx
+++ b/jembatan Beton Coba 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SKRIPSI\Referensi\Jembatan Beton Coba 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikprakoso/Work/Personal/website/flask/f-wbs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9876D8-433C-4E28-ABA3-AE1ABF75B139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84BCE7F-2F2A-6441-B17D-8038BD1DFB79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Floors" sheetId="1" r:id="rId1"/>
@@ -733,7 +733,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -854,16 +854,14 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
@@ -1189,40 +1187,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="3" max="3" width="32.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" hidden="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="54" customHeight="1">
+    <row r="2" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1235,12 +1233,11 @@
       <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:6">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -1253,7 +1250,7 @@
       <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="7" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1265,40 +1262,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" hidden="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="54" customHeight="1">
+    <row r="2" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1311,12 +1308,11 @@
       <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:6">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
@@ -1329,11 +1325,11 @@
       <c r="D3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -1346,11 +1342,11 @@
       <c r="D4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
@@ -1363,11 +1359,11 @@
       <c r="D5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -1380,7 +1376,7 @@
       <c r="D6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="7" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1392,40 +1388,40 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" style="6" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="3" max="3" width="209.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" hidden="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="54" customHeight="1">
+    <row r="2" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1438,110 +1434,109 @@
       <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:6">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>178</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>178</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>177</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="8" t="s">
         <v>177</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="8" t="s">
         <v>177</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="8" t="s">
         <v>177</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="7" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1553,40 +1548,40 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="57.7109375" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="3" max="3" width="57.6640625" customWidth="1"/>
+    <col min="4" max="4" width="28.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" hidden="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="54" customHeight="1">
+    <row r="2" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1599,118 +1594,120 @@
       <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:6">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="9" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="8" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="8" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="8" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="8" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="8" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75">
-      <c r="C9" s="12"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.75">
-      <c r="C10" s="12"/>
-    </row>
-    <row r="11" spans="1:6" ht="15.75">
-      <c r="C11" s="12"/>
-    </row>
-    <row r="12" spans="1:6" ht="15.75">
-      <c r="C12" s="12"/>
-    </row>
-    <row r="13" spans="1:6" ht="15.75">
-      <c r="C13" s="12"/>
-    </row>
-    <row r="14" spans="1:6" ht="15.75">
-      <c r="C14" s="12"/>
-    </row>
-    <row r="15" spans="1:6" ht="15.75">
-      <c r="C15" s="13"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="1"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="C10" s="10"/>
+    </row>
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="C11" s="10"/>
+    </row>
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="C12" s="10"/>
+    </row>
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="C13" s="10"/>
+    </row>
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="C14" s="10"/>
+    </row>
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="C15" s="11"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:E3" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
@@ -1721,40 +1718,40 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" hidden="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="54" customHeight="1">
+    <row r="2" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1767,172 +1764,171 @@
       <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:6">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>175</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>175</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>175</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="8" t="s">
         <v>175</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="9" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="9" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="9" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="9" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="9" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="9" t="s">
         <v>196</v>
       </c>
     </row>
@@ -1945,40 +1941,40 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" hidden="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="54" customHeight="1">
+    <row r="2" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1991,12 +1987,11 @@
       <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:6">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>64</v>
       </c>
@@ -2009,11 +2004,11 @@
       <c r="D3" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="E3" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>68</v>
       </c>
@@ -2026,11 +2021,11 @@
       <c r="D4" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="E4" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>70</v>
       </c>
@@ -2043,11 +2038,11 @@
       <c r="D5" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="E5" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>72</v>
       </c>
@@ -2060,11 +2055,11 @@
       <c r="D6" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="E6" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>74</v>
       </c>
@@ -2077,11 +2072,11 @@
       <c r="D7" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="E7" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>76</v>
       </c>
@@ -2094,11 +2089,11 @@
       <c r="D8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="E8" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>79</v>
       </c>
@@ -2111,11 +2106,11 @@
       <c r="D9" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="E9" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>81</v>
       </c>
@@ -2128,11 +2123,11 @@
       <c r="D10" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="E10" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>83</v>
       </c>
@@ -2145,11 +2140,11 @@
       <c r="D11" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="E11" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>85</v>
       </c>
@@ -2162,11 +2157,11 @@
       <c r="D12" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="E12" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>87</v>
       </c>
@@ -2179,11 +2174,11 @@
       <c r="D13" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="E13" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>89</v>
       </c>
@@ -2196,11 +2191,11 @@
       <c r="D14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="E14" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>91</v>
       </c>
@@ -2213,7 +2208,7 @@
       <c r="D15" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="7" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2225,40 +2220,40 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" hidden="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="54" customHeight="1">
+    <row r="2" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -2271,12 +2266,11 @@
       <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:6">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>93</v>
       </c>
@@ -2289,11 +2283,11 @@
       <c r="D3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="E3" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>95</v>
       </c>
@@ -2306,11 +2300,11 @@
       <c r="D4" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="E4" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>99</v>
       </c>
@@ -2323,11 +2317,11 @@
       <c r="D5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="E5" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>101</v>
       </c>
@@ -2340,11 +2334,11 @@
       <c r="D6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="E6" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>103</v>
       </c>
@@ -2357,11 +2351,11 @@
       <c r="D7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="E7" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>105</v>
       </c>
@@ -2374,11 +2368,11 @@
       <c r="D8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="E8" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>107</v>
       </c>
@@ -2391,11 +2385,11 @@
       <c r="D9" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="E9" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>109</v>
       </c>
@@ -2408,11 +2402,11 @@
       <c r="D10" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="E10" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>111</v>
       </c>
@@ -2425,11 +2419,11 @@
       <c r="D11" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="E11" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>113</v>
       </c>
@@ -2442,11 +2436,11 @@
       <c r="D12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="E12" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>115</v>
       </c>
@@ -2459,11 +2453,11 @@
       <c r="D13" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E13" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="E13" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>119</v>
       </c>
@@ -2476,11 +2470,11 @@
       <c r="D14" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="E14" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>121</v>
       </c>
@@ -2493,11 +2487,11 @@
       <c r="D15" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E15" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="E15" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>123</v>
       </c>
@@ -2510,11 +2504,11 @@
       <c r="D16" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="E16" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>125</v>
       </c>
@@ -2527,11 +2521,11 @@
       <c r="D17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="E17" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>127</v>
       </c>
@@ -2544,11 +2538,11 @@
       <c r="D18" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E18" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="E18" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>129</v>
       </c>
@@ -2561,11 +2555,11 @@
       <c r="D19" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="E19" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>131</v>
       </c>
@@ -2578,11 +2572,11 @@
       <c r="D20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="E20" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>133</v>
       </c>
@@ -2595,11 +2589,11 @@
       <c r="D21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E21" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="E21" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>135</v>
       </c>
@@ -2612,11 +2606,11 @@
       <c r="D22" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="E22" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>137</v>
       </c>
@@ -2629,11 +2623,11 @@
       <c r="D23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="E23" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>139</v>
       </c>
@@ -2646,11 +2640,11 @@
       <c r="D24" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E24" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="E24" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>141</v>
       </c>
@@ -2663,11 +2657,11 @@
       <c r="D25" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="E25" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="E25" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>145</v>
       </c>
@@ -2680,11 +2674,11 @@
       <c r="D26" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E26" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="E26" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>149</v>
       </c>
@@ -2697,11 +2691,11 @@
       <c r="D27" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E27" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="E27" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>151</v>
       </c>
@@ -2714,11 +2708,11 @@
       <c r="D28" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E28" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="E28" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>153</v>
       </c>
@@ -2731,11 +2725,11 @@
       <c r="D29" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E29" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="E29" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>155</v>
       </c>
@@ -2748,11 +2742,11 @@
       <c r="D30" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E30" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="E30" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>157</v>
       </c>
@@ -2765,11 +2759,11 @@
       <c r="D31" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="E31" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>159</v>
       </c>
@@ -2782,11 +2776,11 @@
       <c r="D32" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="E32" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>161</v>
       </c>
@@ -2799,11 +2793,11 @@
       <c r="D33" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="E33" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>163</v>
       </c>
@@ -2816,11 +2810,11 @@
       <c r="D34" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E34" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="E34" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>165</v>
       </c>
@@ -2833,11 +2827,11 @@
       <c r="D35" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E35" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="E35" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>167</v>
       </c>
@@ -2850,11 +2844,11 @@
       <c r="D36" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="E36" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="E36" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>171</v>
       </c>
@@ -2867,11 +2861,11 @@
       <c r="D37" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="E37" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="E37" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>173</v>
       </c>
@@ -2884,7 +2878,7 @@
       <c r="D38" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E38" s="9" t="s">
+      <c r="E38" s="7" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>